<commit_message>
avança nas funções wavelets
</commit_message>
<xml_diff>
--- a/data/processed/BVSP_returns_wide.xlsx
+++ b/data/processed/BVSP_returns_wide.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EF86"/>
+  <dimension ref="A1:EO86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -850,6 +850,33 @@
       <c r="EF1" s="2" t="n">
         <v>45975</v>
       </c>
+      <c r="EG1" s="2" t="n">
+        <v>45978</v>
+      </c>
+      <c r="EH1" s="2" t="n">
+        <v>45979</v>
+      </c>
+      <c r="EI1" s="2" t="n">
+        <v>45980</v>
+      </c>
+      <c r="EJ1" s="2" t="n">
+        <v>45982</v>
+      </c>
+      <c r="EK1" s="2" t="n">
+        <v>45985</v>
+      </c>
+      <c r="EL1" s="2" t="n">
+        <v>45986</v>
+      </c>
+      <c r="EM1" s="2" t="n">
+        <v>45987</v>
+      </c>
+      <c r="EN1" s="2" t="n">
+        <v>45988</v>
+      </c>
+      <c r="EO1" s="2" t="n">
+        <v>45989</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -858,7 +885,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.25901113155597e-05</v>
+        <v>1.249096860986106e-05</v>
       </c>
       <c r="C2" t="n">
         <v>0.0004009204528507837</v>
@@ -1261,6 +1288,33 @@
       </c>
       <c r="EF2" t="n">
         <v>-9.63811323710928e-05</v>
+      </c>
+      <c r="EG2" t="n">
+        <v>-0.0002460859565687201</v>
+      </c>
+      <c r="EH2" t="n">
+        <v>-0.002526920156835644</v>
+      </c>
+      <c r="EI2" t="n">
+        <v>-0.002689254867958013</v>
+      </c>
+      <c r="EJ2" t="n">
+        <v>-0.0003654419906542472</v>
+      </c>
+      <c r="EK2" t="n">
+        <v>-7.064522141853047e-05</v>
+      </c>
+      <c r="EL2" t="n">
+        <v>0.001399050283366066</v>
+      </c>
+      <c r="EM2" t="n">
+        <v>0.002267418008772282</v>
+      </c>
+      <c r="EN2" t="n">
+        <v>-3.742605644063701e-06</v>
+      </c>
+      <c r="EO2" t="n">
+        <v>-0.0001842110058891677</v>
       </c>
     </row>
     <row r="3">
@@ -1674,6 +1728,33 @@
       <c r="EF3" t="n">
         <v>-0.001521733697295247</v>
       </c>
+      <c r="EG3" t="n">
+        <v>0.0007385713067158406</v>
+      </c>
+      <c r="EH3" t="n">
+        <v>-0.0006132245810803738</v>
+      </c>
+      <c r="EI3" t="n">
+        <v>0.0003056703984825049</v>
+      </c>
+      <c r="EJ3" t="n">
+        <v>-0.002020590393826183</v>
+      </c>
+      <c r="EK3" t="n">
+        <v>-0.0008096202274803233</v>
+      </c>
+      <c r="EL3" t="n">
+        <v>0.00155646475526261</v>
+      </c>
+      <c r="EM3" t="n">
+        <v>-0.001565012909939156</v>
+      </c>
+      <c r="EN3" t="n">
+        <v>-0.0001932556731283341</v>
+      </c>
+      <c r="EO3" t="n">
+        <v>0.002906022822960708</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -2086,6 +2167,33 @@
       <c r="EF4" t="n">
         <v>0.0003598516963556619</v>
       </c>
+      <c r="EG4" t="n">
+        <v>-0.000104656361624933</v>
+      </c>
+      <c r="EH4" t="n">
+        <v>-0.000158852517898822</v>
+      </c>
+      <c r="EI4" t="n">
+        <v>-0.0003618486238661234</v>
+      </c>
+      <c r="EJ4" t="n">
+        <v>9.196114406151423e-05</v>
+      </c>
+      <c r="EK4" t="n">
+        <v>0.001131144416461893</v>
+      </c>
+      <c r="EL4" t="n">
+        <v>0.001169867782621736</v>
+      </c>
+      <c r="EM4" t="n">
+        <v>0.0002024810026064472</v>
+      </c>
+      <c r="EN4" t="n">
+        <v>0.0005556324948248204</v>
+      </c>
+      <c r="EO4" t="n">
+        <v>0.0004745188208588047</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -2498,6 +2606,33 @@
       <c r="EF5" t="n">
         <v>0.00112137626442177</v>
       </c>
+      <c r="EG5" t="n">
+        <v>-0.0002840234455288027</v>
+      </c>
+      <c r="EH5" t="n">
+        <v>0.003271674162911964</v>
+      </c>
+      <c r="EI5" t="n">
+        <v>-0.001106883828549954</v>
+      </c>
+      <c r="EJ5" t="n">
+        <v>-0.00101203801116867</v>
+      </c>
+      <c r="EK5" t="n">
+        <v>-0.0001735738687127508</v>
+      </c>
+      <c r="EL5" t="n">
+        <v>0.001001598496234379</v>
+      </c>
+      <c r="EM5" t="n">
+        <v>0.001815199719301219</v>
+      </c>
+      <c r="EN5" t="n">
+        <v>-0.0001675829578946519</v>
+      </c>
+      <c r="EO5" t="n">
+        <v>0.0009728265475121844</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -2910,6 +3045,33 @@
       <c r="EF6" t="n">
         <v>0.0004489546953561074</v>
       </c>
+      <c r="EG6" t="n">
+        <v>0.0003353133621892823</v>
+      </c>
+      <c r="EH6" t="n">
+        <v>0.0008533068302423175</v>
+      </c>
+      <c r="EI6" t="n">
+        <v>0.0009804963198742911</v>
+      </c>
+      <c r="EJ6" t="n">
+        <v>-5.692729477502212e-05</v>
+      </c>
+      <c r="EK6" t="n">
+        <v>-9.624096239946311e-05</v>
+      </c>
+      <c r="EL6" t="n">
+        <v>0.0008321333365852723</v>
+      </c>
+      <c r="EM6" t="n">
+        <v>0.001950601214918635</v>
+      </c>
+      <c r="EN6" t="n">
+        <v>0.001060065015082046</v>
+      </c>
+      <c r="EO6" t="n">
+        <v>-0.00100370670173433</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -3322,6 +3484,33 @@
       <c r="EF7" t="n">
         <v>-0.0008712276589903922</v>
       </c>
+      <c r="EG7" t="n">
+        <v>-0.0005587859930713535</v>
+      </c>
+      <c r="EH7" t="n">
+        <v>0.001029888350201347</v>
+      </c>
+      <c r="EI7" t="n">
+        <v>-0.0007486376437650932</v>
+      </c>
+      <c r="EJ7" t="n">
+        <v>-0.001193999120356892</v>
+      </c>
+      <c r="EK7" t="n">
+        <v>0.001338160221076024</v>
+      </c>
+      <c r="EL7" t="n">
+        <v>0.0001278744828212552</v>
+      </c>
+      <c r="EM7" t="n">
+        <v>0.001278570451841432</v>
+      </c>
+      <c r="EN7" t="n">
+        <v>-0.0001618256454687383</v>
+      </c>
+      <c r="EO7" t="n">
+        <v>-0.0006507702215472477</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -3734,6 +3923,33 @@
       <c r="EF8" t="n">
         <v>0.001299198668721857</v>
       </c>
+      <c r="EG8" t="n">
+        <v>-0.001885556205817096</v>
+      </c>
+      <c r="EH8" t="n">
+        <v>-0.0007081276216354127</v>
+      </c>
+      <c r="EI8" t="n">
+        <v>0.0003122676620197495</v>
+      </c>
+      <c r="EJ8" t="n">
+        <v>0.0006121253644835178</v>
+      </c>
+      <c r="EK8" t="n">
+        <v>0.001821635823993972</v>
+      </c>
+      <c r="EL8" t="n">
+        <v>-0.0004523831338243411</v>
+      </c>
+      <c r="EM8" t="n">
+        <v>0.000273390524355932</v>
+      </c>
+      <c r="EN8" t="n">
+        <v>-0.001198521379910389</v>
+      </c>
+      <c r="EO8" t="n">
+        <v>-0.0004928602060534359</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -4146,6 +4362,33 @@
       <c r="EF9" t="n">
         <v>-0.001785302081479756</v>
       </c>
+      <c r="EG9" t="n">
+        <v>-0.001048385042478728</v>
+      </c>
+      <c r="EH9" t="n">
+        <v>-0.0009706869402528184</v>
+      </c>
+      <c r="EI9" t="n">
+        <v>0.0003948048304422969</v>
+      </c>
+      <c r="EJ9" t="n">
+        <v>0.001507246902026083</v>
+      </c>
+      <c r="EK9" t="n">
+        <v>0.0001686140927219526</v>
+      </c>
+      <c r="EL9" t="n">
+        <v>-0.0007072836247434822</v>
+      </c>
+      <c r="EM9" t="n">
+        <v>0.0009696849065559121</v>
+      </c>
+      <c r="EN9" t="n">
+        <v>1.891185891800262e-05</v>
+      </c>
+      <c r="EO9" t="n">
+        <v>0.000150531707513224</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -4558,6 +4801,33 @@
       <c r="EF10" t="n">
         <v>0.0009410199483976811</v>
       </c>
+      <c r="EG10" t="n">
+        <v>-0.001489907210121544</v>
+      </c>
+      <c r="EH10" t="n">
+        <v>0.0001791732746188046</v>
+      </c>
+      <c r="EI10" t="n">
+        <v>-0.0002480246194185298</v>
+      </c>
+      <c r="EJ10" t="n">
+        <v>0.0002110451223416021</v>
+      </c>
+      <c r="EK10" t="n">
+        <v>-0.001292158559186518</v>
+      </c>
+      <c r="EL10" t="n">
+        <v>-0.002406446273484519</v>
+      </c>
+      <c r="EM10" t="n">
+        <v>0.0005219091509101048</v>
+      </c>
+      <c r="EN10" t="n">
+        <v>-0.0003526862214862092</v>
+      </c>
+      <c r="EO10" t="n">
+        <v>-0.0007521956134066698</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -4970,6 +5240,33 @@
       <c r="EF11" t="n">
         <v>-0.0008431030433158071</v>
       </c>
+      <c r="EG11" t="n">
+        <v>0.0009286684947653612</v>
+      </c>
+      <c r="EH11" t="n">
+        <v>2.526544319181312e-05</v>
+      </c>
+      <c r="EI11" t="n">
+        <v>-0.0004763877990914267</v>
+      </c>
+      <c r="EJ11" t="n">
+        <v>-0.001385765701311215</v>
+      </c>
+      <c r="EK11" t="n">
+        <v>-0.0001854648949990434</v>
+      </c>
+      <c r="EL11" t="n">
+        <v>-0.002364580703799746</v>
+      </c>
+      <c r="EM11" t="n">
+        <v>-0.0004802020018228603</v>
+      </c>
+      <c r="EN11" t="n">
+        <v>-3.596522055282492e-05</v>
+      </c>
+      <c r="EO11" t="n">
+        <v>-0.000142860943341816</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -5382,6 +5679,33 @@
       <c r="EF12" t="n">
         <v>-0.001111815716582143</v>
       </c>
+      <c r="EG12" t="n">
+        <v>-0.0006772451082515119</v>
+      </c>
+      <c r="EH12" t="n">
+        <v>0.001716853383440409</v>
+      </c>
+      <c r="EI12" t="n">
+        <v>0.0001551465667120056</v>
+      </c>
+      <c r="EJ12" t="n">
+        <v>-0.0001795282652281571</v>
+      </c>
+      <c r="EK12" t="n">
+        <v>-0.0001967916713478957</v>
+      </c>
+      <c r="EL12" t="n">
+        <v>0.0001010660660689666</v>
+      </c>
+      <c r="EM12" t="n">
+        <v>0.001224520875311441</v>
+      </c>
+      <c r="EN12" t="n">
+        <v>5.518035651519426e-06</v>
+      </c>
+      <c r="EO12" t="n">
+        <v>0.0002013787753387675</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -5794,6 +6118,33 @@
       <c r="EF13" t="n">
         <v>0.001951734068073918</v>
       </c>
+      <c r="EG13" t="n">
+        <v>0.0008523989150148736</v>
+      </c>
+      <c r="EH13" t="n">
+        <v>-0.0008744716003441511</v>
+      </c>
+      <c r="EI13" t="n">
+        <v>0.000108928974256628</v>
+      </c>
+      <c r="EJ13" t="n">
+        <v>-7.614264206701193e-05</v>
+      </c>
+      <c r="EK13" t="n">
+        <v>-0.0008728223433767113</v>
+      </c>
+      <c r="EL13" t="n">
+        <v>-0.000348695956603251</v>
+      </c>
+      <c r="EM13" t="n">
+        <v>0.0006003494699946543</v>
+      </c>
+      <c r="EN13" t="n">
+        <v>-0.0009119729881295058</v>
+      </c>
+      <c r="EO13" t="n">
+        <v>0.0005523026719558288</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -6206,6 +6557,33 @@
       <c r="EF14" t="n">
         <v>-0.001087468416518078</v>
       </c>
+      <c r="EG14" t="n">
+        <v>-0.000698810032956132</v>
+      </c>
+      <c r="EH14" t="n">
+        <v>0.0001063577596660537</v>
+      </c>
+      <c r="EI14" t="n">
+        <v>-6.012313207293118e-07</v>
+      </c>
+      <c r="EJ14" t="n">
+        <v>-0.000119375864342075</v>
+      </c>
+      <c r="EK14" t="n">
+        <v>0.0004610677785734651</v>
+      </c>
+      <c r="EL14" t="n">
+        <v>0.0004456293325798555</v>
+      </c>
+      <c r="EM14" t="n">
+        <v>0.0005927578484339335</v>
+      </c>
+      <c r="EN14" t="n">
+        <v>0.0002675364988053985</v>
+      </c>
+      <c r="EO14" t="n">
+        <v>0.0007605909551848811</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -6618,6 +6996,33 @@
       <c r="EF15" t="n">
         <v>0.0005062914261966256</v>
       </c>
+      <c r="EG15" t="n">
+        <v>0.0007229633438612382</v>
+      </c>
+      <c r="EH15" t="n">
+        <v>-9.069272637063364e-05</v>
+      </c>
+      <c r="EI15" t="n">
+        <v>0.0002800344615980777</v>
+      </c>
+      <c r="EJ15" t="n">
+        <v>-0.002045337219424681</v>
+      </c>
+      <c r="EK15" t="n">
+        <v>-0.0003720661497439437</v>
+      </c>
+      <c r="EL15" t="n">
+        <v>-0.0007208903141222578</v>
+      </c>
+      <c r="EM15" t="n">
+        <v>-0.0006095092044393624</v>
+      </c>
+      <c r="EN15" t="n">
+        <v>-0.001075905813960887</v>
+      </c>
+      <c r="EO15" t="n">
+        <v>-0.001090379808129427</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -7030,6 +7435,33 @@
       <c r="EF16" t="n">
         <v>0.001643107443957348</v>
       </c>
+      <c r="EG16" t="n">
+        <v>0.001465600180976523</v>
+      </c>
+      <c r="EH16" t="n">
+        <v>-0.001044307072042727</v>
+      </c>
+      <c r="EI16" t="n">
+        <v>6.78176602750824e-05</v>
+      </c>
+      <c r="EJ16" t="n">
+        <v>-0.001778482917874413</v>
+      </c>
+      <c r="EK16" t="n">
+        <v>0.001150354417724486</v>
+      </c>
+      <c r="EL16" t="n">
+        <v>-8.11037598289488e-05</v>
+      </c>
+      <c r="EM16" t="n">
+        <v>5.05505750680868e-05</v>
+      </c>
+      <c r="EN16" t="n">
+        <v>-2.892120024355904e-05</v>
+      </c>
+      <c r="EO16" t="n">
+        <v>0.001537626076487442</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -7442,6 +7874,33 @@
       <c r="EF17" t="n">
         <v>0.001007472662044151</v>
       </c>
+      <c r="EG17" t="n">
+        <v>0.0009914086342792672</v>
+      </c>
+      <c r="EH17" t="n">
+        <v>0.0004121229307063601</v>
+      </c>
+      <c r="EI17" t="n">
+        <v>-0.001047629762288338</v>
+      </c>
+      <c r="EJ17" t="n">
+        <v>-0.0006696877409151369</v>
+      </c>
+      <c r="EK17" t="n">
+        <v>0.0005640542246148073</v>
+      </c>
+      <c r="EL17" t="n">
+        <v>-0.001173419635534856</v>
+      </c>
+      <c r="EM17" t="n">
+        <v>0.000639293778542438</v>
+      </c>
+      <c r="EN17" t="n">
+        <v>0.0003671285751156717</v>
+      </c>
+      <c r="EO17" t="n">
+        <v>0.001457595779680076</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -7854,6 +8313,33 @@
       <c r="EF18" t="n">
         <v>0.0005126372947312774</v>
       </c>
+      <c r="EG18" t="n">
+        <v>-0.0001360447355267524</v>
+      </c>
+      <c r="EH18" t="n">
+        <v>-0.000443885514386011</v>
+      </c>
+      <c r="EI18" t="n">
+        <v>0.0007038860472423636</v>
+      </c>
+      <c r="EJ18" t="n">
+        <v>0.0001337096819877814</v>
+      </c>
+      <c r="EK18" t="n">
+        <v>0.0008191155329768662</v>
+      </c>
+      <c r="EL18" t="n">
+        <v>-0.001592671066813267</v>
+      </c>
+      <c r="EM18" t="n">
+        <v>9.707139561498934e-06</v>
+      </c>
+      <c r="EN18" t="n">
+        <v>-1.894527322399142e-05</v>
+      </c>
+      <c r="EO18" t="n">
+        <v>0.000178994394653742</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -8266,6 +8752,33 @@
       <c r="EF19" t="n">
         <v>0.0007047326430758005</v>
       </c>
+      <c r="EG19" t="n">
+        <v>0.0006740928155881676</v>
+      </c>
+      <c r="EH19" t="n">
+        <v>0.0002358980044707693</v>
+      </c>
+      <c r="EI19" t="n">
+        <v>0.0006112630665988661</v>
+      </c>
+      <c r="EJ19" t="n">
+        <v>0.001957134210430311</v>
+      </c>
+      <c r="EK19" t="n">
+        <v>0.002542281183396611</v>
+      </c>
+      <c r="EL19" t="n">
+        <v>0.0002660585440334984</v>
+      </c>
+      <c r="EM19" t="n">
+        <v>-0.000413231109014589</v>
+      </c>
+      <c r="EN19" t="n">
+        <v>1.894527322399142e-05</v>
+      </c>
+      <c r="EO19" t="n">
+        <v>-0.0003295394431379606</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -8678,6 +9191,33 @@
       <c r="EF20" t="n">
         <v>-0.00144274342777706</v>
       </c>
+      <c r="EG20" t="n">
+        <v>-0.001336633383729691</v>
+      </c>
+      <c r="EH20" t="n">
+        <v>0.0007073603098657344</v>
+      </c>
+      <c r="EI20" t="n">
+        <v>9.703444615283274e-05</v>
+      </c>
+      <c r="EJ20" t="n">
+        <v>0.001807895215556243</v>
+      </c>
+      <c r="EK20" t="n">
+        <v>0.0002421198386581835</v>
+      </c>
+      <c r="EL20" t="n">
+        <v>0.001530403427166149</v>
+      </c>
+      <c r="EM20" t="n">
+        <v>0.0008587666282338091</v>
+      </c>
+      <c r="EN20" t="n">
+        <v>-4.045575080269259e-06</v>
+      </c>
+      <c r="EO20" t="n">
+        <v>-0.001738457504599111</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -9090,6 +9630,33 @@
       <c r="EF21" t="n">
         <v>0.002177113433120326</v>
       </c>
+      <c r="EG21" t="n">
+        <v>-0.000586723208501283</v>
+      </c>
+      <c r="EH21" t="n">
+        <v>0.0006303727223748723</v>
+      </c>
+      <c r="EI21" t="n">
+        <v>0.0006836806991081801</v>
+      </c>
+      <c r="EJ21" t="n">
+        <v>-0.0009092541674178278</v>
+      </c>
+      <c r="EK21" t="n">
+        <v>-0.002077289450674868</v>
+      </c>
+      <c r="EL21" t="n">
+        <v>0.001169558751277222</v>
+      </c>
+      <c r="EM21" t="n">
+        <v>-0.001049835998889748</v>
+      </c>
+      <c r="EN21" t="n">
+        <v>0.0002213971689730698</v>
+      </c>
+      <c r="EO21" t="n">
+        <v>-0.001415033345850247</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -9502,6 +10069,33 @@
       <c r="EF22" t="n">
         <v>0.0001611600194610929</v>
       </c>
+      <c r="EG22" t="n">
+        <v>0.0005767008840216192</v>
+      </c>
+      <c r="EH22" t="n">
+        <v>-0.00141372965786779</v>
+      </c>
+      <c r="EI22" t="n">
+        <v>-0.0001806344557486739</v>
+      </c>
+      <c r="EJ22" t="n">
+        <v>-0.0006071014049826573</v>
+      </c>
+      <c r="EK22" t="n">
+        <v>0.0001621184663118669</v>
+      </c>
+      <c r="EL22" t="n">
+        <v>-0.001155457110883162</v>
+      </c>
+      <c r="EM22" t="n">
+        <v>0.0003790309428275407</v>
+      </c>
+      <c r="EN22" t="n">
+        <v>-0.0002015641403794177</v>
+      </c>
+      <c r="EO22" t="n">
+        <v>-0.0001778452948659748</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -9914,6 +10508,33 @@
       <c r="EF23" t="n">
         <v>0.001603741740211717</v>
       </c>
+      <c r="EG23" t="n">
+        <v>8.692295714318732e-05</v>
+      </c>
+      <c r="EH23" t="n">
+        <v>0.000697134871913363</v>
+      </c>
+      <c r="EI23" t="n">
+        <v>-0.0002834767318820042</v>
+      </c>
+      <c r="EJ23" t="n">
+        <v>-0.001062099280948914</v>
+      </c>
+      <c r="EK23" t="n">
+        <v>-0.0003148074063474837</v>
+      </c>
+      <c r="EL23" t="n">
+        <v>-0.001958707274887672</v>
+      </c>
+      <c r="EM23" t="n">
+        <v>-0.0002634732156181485</v>
+      </c>
+      <c r="EN23" t="n">
+        <v>8.97900299712262e-06</v>
+      </c>
+      <c r="EO23" t="n">
+        <v>8.395086159929122e-05</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -10326,6 +10947,33 @@
       <c r="EF24" t="n">
         <v>0.0005177576954302765</v>
       </c>
+      <c r="EG24" t="n">
+        <v>0.001228615528820143</v>
+      </c>
+      <c r="EH24" t="n">
+        <v>-0.001130455928937124</v>
+      </c>
+      <c r="EI24" t="n">
+        <v>-0.0003629715221364904</v>
+      </c>
+      <c r="EJ24" t="n">
+        <v>-0.0001911112598627085</v>
+      </c>
+      <c r="EK24" t="n">
+        <v>0.0002778000467049679</v>
+      </c>
+      <c r="EL24" t="n">
+        <v>0.002017931993126609</v>
+      </c>
+      <c r="EM24" t="n">
+        <v>-0.0003143958432083593</v>
+      </c>
+      <c r="EN24" t="n">
+        <v>-0.0003494512363353408</v>
+      </c>
+      <c r="EO24" t="n">
+        <v>0.0009365790929329876</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -10738,6 +11386,33 @@
       <c r="EF25" t="n">
         <v>0.0006837336034610786</v>
       </c>
+      <c r="EG25" t="n">
+        <v>0.0001441815250871059</v>
+      </c>
+      <c r="EH25" t="n">
+        <v>-0.0004005244445401956</v>
+      </c>
+      <c r="EI25" t="n">
+        <v>0.001404393761850642</v>
+      </c>
+      <c r="EJ25" t="n">
+        <v>-0.0003600287818645853</v>
+      </c>
+      <c r="EK25" t="n">
+        <v>-0.0004345366579912024</v>
+      </c>
+      <c r="EL25" t="n">
+        <v>0.0003491329539695442</v>
+      </c>
+      <c r="EM25" t="n">
+        <v>-0.0005185924426900357</v>
+      </c>
+      <c r="EN25" t="n">
+        <v>-0.0003509557409753228</v>
+      </c>
+      <c r="EO25" t="n">
+        <v>0.000644262740753021</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -11150,6 +11825,33 @@
       <c r="EF26" t="n">
         <v>-0.001476207576400768</v>
       </c>
+      <c r="EG26" t="n">
+        <v>0.0009617681824458657</v>
+      </c>
+      <c r="EH26" t="n">
+        <v>-0.001015820708509807</v>
+      </c>
+      <c r="EI26" t="n">
+        <v>-0.0004764501622798178</v>
+      </c>
+      <c r="EJ26" t="n">
+        <v>4.034751170500783e-05</v>
+      </c>
+      <c r="EK26" t="n">
+        <v>0.0007630296578469142</v>
+      </c>
+      <c r="EL26" t="n">
+        <v>-0.0006684642025103216</v>
+      </c>
+      <c r="EM26" t="n">
+        <v>-0.0004768862307020783</v>
+      </c>
+      <c r="EN26" t="n">
+        <v>0.0001400021762858472</v>
+      </c>
+      <c r="EO26" t="n">
+        <v>-0.00139847991531461</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -11562,6 +12264,33 @@
       <c r="EF27" t="n">
         <v>0.0004232256018372738</v>
       </c>
+      <c r="EG27" t="n">
+        <v>-0.0005184535309084026</v>
+      </c>
+      <c r="EH27" t="n">
+        <v>0.0007702102936733013</v>
+      </c>
+      <c r="EI27" t="n">
+        <v>-0.0004300303344226819</v>
+      </c>
+      <c r="EJ27" t="n">
+        <v>0.0008069124345073675</v>
+      </c>
+      <c r="EK27" t="n">
+        <v>6.675122494392838e-05</v>
+      </c>
+      <c r="EL27" t="n">
+        <v>0.002341341210570391</v>
+      </c>
+      <c r="EM27" t="n">
+        <v>0.0005178479585179474</v>
+      </c>
+      <c r="EN27" t="n">
+        <v>-6.091532234009378e-05</v>
+      </c>
+      <c r="EO27" t="n">
+        <v>3.684272432380453e-05</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -11974,6 +12703,33 @@
       <c r="EF28" t="n">
         <v>5.579660437504685e-05</v>
       </c>
+      <c r="EG28" t="n">
+        <v>-0.0007904755739218672</v>
+      </c>
+      <c r="EH28" t="n">
+        <v>0.0001064685759004647</v>
+      </c>
+      <c r="EI28" t="n">
+        <v>0.000116607833225757</v>
+      </c>
+      <c r="EJ28" t="n">
+        <v>-0.0008825400090870517</v>
+      </c>
+      <c r="EK28" t="n">
+        <v>0.0002801256030355859</v>
+      </c>
+      <c r="EL28" t="n">
+        <v>-0.0006031766244056769</v>
+      </c>
+      <c r="EM28" t="n">
+        <v>-0.0002814101533825664</v>
+      </c>
+      <c r="EN28" t="n">
+        <v>0.0003659297620544066</v>
+      </c>
+      <c r="EO28" t="n">
+        <v>0.0003219712825295318</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -12386,6 +13142,33 @@
       <c r="EF29" t="n">
         <v>0.0006048569523695591</v>
       </c>
+      <c r="EG29" t="n">
+        <v>0.0003047509205149623</v>
+      </c>
+      <c r="EH29" t="n">
+        <v>0.000158632145433657</v>
+      </c>
+      <c r="EI29" t="n">
+        <v>-0.001025814380117396</v>
+      </c>
+      <c r="EJ29" t="n">
+        <v>-0.0003379609065241596</v>
+      </c>
+      <c r="EK29" t="n">
+        <v>-0.0005568103226654131</v>
+      </c>
+      <c r="EL29" t="n">
+        <v>0.001489032631228682</v>
+      </c>
+      <c r="EM29" t="n">
+        <v>-0.0004200306764516881</v>
+      </c>
+      <c r="EN29" t="n">
+        <v>0.0001584918057329077</v>
+      </c>
+      <c r="EO29" t="n">
+        <v>5.731164092637187e-05</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -12798,6 +13581,33 @@
       <c r="EF30" t="n">
         <v>-0.0006057472992733182</v>
       </c>
+      <c r="EG30" t="n">
+        <v>0.001233910915891201</v>
+      </c>
+      <c r="EH30" t="n">
+        <v>0.001112117100179333</v>
+      </c>
+      <c r="EI30" t="n">
+        <v>-0.000744684809248497</v>
+      </c>
+      <c r="EJ30" t="n">
+        <v>-0.001317647192157878</v>
+      </c>
+      <c r="EK30" t="n">
+        <v>-8.436787475396557e-05</v>
+      </c>
+      <c r="EL30" t="n">
+        <v>-0.001341196068201711</v>
+      </c>
+      <c r="EM30" t="n">
+        <v>-0.0004933867416188065</v>
+      </c>
+      <c r="EN30" t="n">
+        <v>-0.0001744805433450125</v>
+      </c>
+      <c r="EO30" t="n">
+        <v>-0.0004586836392057592</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -13210,6 +14020,33 @@
       <c r="EF31" t="n">
         <v>0.0008324249458997457</v>
       </c>
+      <c r="EG31" t="n">
+        <v>-0.0004502109623221173</v>
+      </c>
+      <c r="EH31" t="n">
+        <v>0.0003831057022285478</v>
+      </c>
+      <c r="EI31" t="n">
+        <v>4.832612152227966e-05</v>
+      </c>
+      <c r="EJ31" t="n">
+        <v>0.0002494754251483045</v>
+      </c>
+      <c r="EK31" t="n">
+        <v>-0.0001097190514549595</v>
+      </c>
+      <c r="EL31" t="n">
+        <v>0.0008097967346216706</v>
+      </c>
+      <c r="EM31" t="n">
+        <v>0.0001024697494198534</v>
+      </c>
+      <c r="EN31" t="n">
+        <v>9.523778043529774e-05</v>
+      </c>
+      <c r="EO31" t="n">
+        <v>0.0001725850776299609</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -13622,6 +14459,33 @@
       <c r="EF32" t="n">
         <v>0.0001884799610696319</v>
       </c>
+      <c r="EG32" t="n">
+        <v>-0.0009832889238392539</v>
+      </c>
+      <c r="EH32" t="n">
+        <v>-0.0003404756900451389</v>
+      </c>
+      <c r="EI32" t="n">
+        <v>-0.0004573869805692965</v>
+      </c>
+      <c r="EJ32" t="n">
+        <v>0.0002981313520589168</v>
+      </c>
+      <c r="EK32" t="n">
+        <v>0.0001111269170586127</v>
+      </c>
+      <c r="EL32" t="n">
+        <v>0.001318235538883883</v>
+      </c>
+      <c r="EM32" t="n">
+        <v>-0.000680846204376806</v>
+      </c>
+      <c r="EN32" t="n">
+        <v>0.0001933097371225045</v>
+      </c>
+      <c r="EO32" t="n">
+        <v>0.0008407291454677335</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
@@ -14034,6 +14898,33 @@
       <c r="EF33" t="n">
         <v>-0.0001984633722980078</v>
       </c>
+      <c r="EG33" t="n">
+        <v>0.0009213046998937102</v>
+      </c>
+      <c r="EH33" t="n">
+        <v>-0.0007092723016022262</v>
+      </c>
+      <c r="EI33" t="n">
+        <v>0.0002564472759409853</v>
+      </c>
+      <c r="EJ33" t="n">
+        <v>-0.002389476228222165</v>
+      </c>
+      <c r="EK33" t="n">
+        <v>-0.0004547430883050652</v>
+      </c>
+      <c r="EL33" t="n">
+        <v>-0.0001123959485660464</v>
+      </c>
+      <c r="EM33" t="n">
+        <v>0.001199587095113586</v>
+      </c>
+      <c r="EN33" t="n">
+        <v>-4.262558192813515e-05</v>
+      </c>
+      <c r="EO33" t="n">
+        <v>0.0003185224678006193</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -14446,6 +15337,33 @@
       <c r="EF34" t="n">
         <v>-9.242542053655711e-05</v>
       </c>
+      <c r="EG34" t="n">
+        <v>0.0001719819097480979</v>
+      </c>
+      <c r="EH34" t="n">
+        <v>0.0009260881697787937</v>
+      </c>
+      <c r="EI34" t="n">
+        <v>-0.0004205598984956538</v>
+      </c>
+      <c r="EJ34" t="n">
+        <v>0.002069415465715707</v>
+      </c>
+      <c r="EK34" t="n">
+        <v>-7.213817814566426e-05</v>
+      </c>
+      <c r="EL34" t="n">
+        <v>6.96468353780233e-05</v>
+      </c>
+      <c r="EM34" t="n">
+        <v>0.0002349628034341578</v>
+      </c>
+      <c r="EN34" t="n">
+        <v>1.864891566327742e-05</v>
+      </c>
+      <c r="EO34" t="n">
+        <v>-0.0001377482705660071</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -14858,6 +15776,33 @@
       <c r="EF35" t="n">
         <v>0.0009880645579158909</v>
       </c>
+      <c r="EG35" t="n">
+        <v>-0.0007289230643401368</v>
+      </c>
+      <c r="EH35" t="n">
+        <v>-0.001056672270047798</v>
+      </c>
+      <c r="EI35" t="n">
+        <v>0.0003674104102326936</v>
+      </c>
+      <c r="EJ35" t="n">
+        <v>0.001300921877666283</v>
+      </c>
+      <c r="EK35" t="n">
+        <v>0.0007075744197528877</v>
+      </c>
+      <c r="EL35" t="n">
+        <v>-0.0009457645915968982</v>
+      </c>
+      <c r="EM35" t="n">
+        <v>0.0004406048478688973</v>
+      </c>
+      <c r="EN35" t="n">
+        <v>-0.0002250929504743482</v>
+      </c>
+      <c r="EO35" t="n">
+        <v>-0.0001253674182155606</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -15270,6 +16215,33 @@
       <c r="EF36" t="n">
         <v>-0.001093153247973433</v>
       </c>
+      <c r="EG36" t="n">
+        <v>0.0008668238610223256</v>
+      </c>
+      <c r="EH36" t="n">
+        <v>0.0001128008876207787</v>
+      </c>
+      <c r="EI36" t="n">
+        <v>-0.0006754450702803894</v>
+      </c>
+      <c r="EJ36" t="n">
+        <v>-0.000809452993983939</v>
+      </c>
+      <c r="EK36" t="n">
+        <v>-0.0005320170813458702</v>
+      </c>
+      <c r="EL36" t="n">
+        <v>-0.001244409877838137</v>
+      </c>
+      <c r="EM36" t="n">
+        <v>0.0008678461294024942</v>
+      </c>
+      <c r="EN36" t="n">
+        <v>0.0001847358642592667</v>
+      </c>
+      <c r="EO36" t="n">
+        <v>-8.699887448315735e-05</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -15682,6 +16654,33 @@
       <c r="EF37" t="n">
         <v>0.0002017644859737544</v>
       </c>
+      <c r="EG37" t="n">
+        <v>-0.001511908222298075</v>
+      </c>
+      <c r="EH37" t="n">
+        <v>0.0001304694785186911</v>
+      </c>
+      <c r="EI37" t="n">
+        <v>-0.0001367897828679077</v>
+      </c>
+      <c r="EJ37" t="n">
+        <v>-4.982609324422071e-05</v>
+      </c>
+      <c r="EK37" t="n">
+        <v>-0.0004418194278112964</v>
+      </c>
+      <c r="EL37" t="n">
+        <v>-0.0004557965228624283</v>
+      </c>
+      <c r="EM37" t="n">
+        <v>0.0002468837869535889</v>
+      </c>
+      <c r="EN37" t="n">
+        <v>-9.078101969706154e-06</v>
+      </c>
+      <c r="EO37" t="n">
+        <v>0.0005980136444261319</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -16094,6 +17093,33 @@
       <c r="EF38" t="n">
         <v>-0.001117086217591989</v>
       </c>
+      <c r="EG38" t="n">
+        <v>0.0002483111016786665</v>
+      </c>
+      <c r="EH38" t="n">
+        <v>0.0003602511130011976</v>
+      </c>
+      <c r="EI38" t="n">
+        <v>-2.308425408159565e-06</v>
+      </c>
+      <c r="EJ38" t="n">
+        <v>-0.0009168981425027312</v>
+      </c>
+      <c r="EK38" t="n">
+        <v>0.0001068756142963423</v>
+      </c>
+      <c r="EL38" t="n">
+        <v>-0.000913324580332997</v>
+      </c>
+      <c r="EM38" t="n">
+        <v>0.001374083943842308</v>
+      </c>
+      <c r="EN38" t="n">
+        <v>-0.0001076607322243461</v>
+      </c>
+      <c r="EO38" t="n">
+        <v>0.001029009312802032</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -16506,6 +17532,33 @@
       <c r="EF39" t="n">
         <v>0.0005560782156823763</v>
       </c>
+      <c r="EG39" t="n">
+        <v>0.0002265486707297981</v>
+      </c>
+      <c r="EH39" t="n">
+        <v>0.0003554297522541106</v>
+      </c>
+      <c r="EI39" t="n">
+        <v>-0.0004672145295341323</v>
+      </c>
+      <c r="EJ39" t="n">
+        <v>0.0003834714899983993</v>
+      </c>
+      <c r="EK39" t="n">
+        <v>-0.0003397872819395076</v>
+      </c>
+      <c r="EL39" t="n">
+        <v>0.0004541996249649571</v>
+      </c>
+      <c r="EM39" t="n">
+        <v>2.641190292607121e-05</v>
+      </c>
+      <c r="EN39" t="n">
+        <v>0.000203864687049915</v>
+      </c>
+      <c r="EO39" t="n">
+        <v>-0.0003809255790603316</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -16918,6 +17971,33 @@
       <c r="EF40" t="n">
         <v>0.000150714067515878</v>
       </c>
+      <c r="EG40" t="n">
+        <v>-0.0001762000860594526</v>
+      </c>
+      <c r="EH40" t="n">
+        <v>0.000325367033848778</v>
+      </c>
+      <c r="EI40" t="n">
+        <v>-0.0001729267249910293</v>
+      </c>
+      <c r="EJ40" t="n">
+        <v>-0.000239957127726953</v>
+      </c>
+      <c r="EK40" t="n">
+        <v>2.516621657733253e-06</v>
+      </c>
+      <c r="EL40" t="n">
+        <v>0.000147764220914226</v>
+      </c>
+      <c r="EM40" t="n">
+        <v>0.000623395301449392</v>
+      </c>
+      <c r="EN40" t="n">
+        <v>0.00062889647119313</v>
+      </c>
+      <c r="EO40" t="n">
+        <v>-0.000261503501114646</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
@@ -17330,6 +18410,33 @@
       <c r="EF41" t="n">
         <v>-0.0001119455494862365</v>
       </c>
+      <c r="EG41" t="n">
+        <v>7.898666749817096e-05</v>
+      </c>
+      <c r="EH41" t="n">
+        <v>-4.340941974234624e-05</v>
+      </c>
+      <c r="EI41" t="n">
+        <v>5.091707222071307e-05</v>
+      </c>
+      <c r="EJ41" t="n">
+        <v>-0.0006238735924242178</v>
+      </c>
+      <c r="EK41" t="n">
+        <v>0.0008528705354251542</v>
+      </c>
+      <c r="EL41" t="n">
+        <v>0.0004184126162840585</v>
+      </c>
+      <c r="EM41" t="n">
+        <v>0.0001885044981015938</v>
+      </c>
+      <c r="EN41" t="n">
+        <v>9.702157574054127e-05</v>
+      </c>
+      <c r="EO41" t="n">
+        <v>-6.076511541586171e-05</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
@@ -17742,6 +18849,33 @@
       <c r="EF42" t="n">
         <v>-1.206555115018659e-05</v>
       </c>
+      <c r="EG42" t="n">
+        <v>0.000235832721971363</v>
+      </c>
+      <c r="EH42" t="n">
+        <v>0.0005943955796663403</v>
+      </c>
+      <c r="EI42" t="n">
+        <v>-8.134506169099609e-06</v>
+      </c>
+      <c r="EJ42" t="n">
+        <v>0.001436123967941683</v>
+      </c>
+      <c r="EK42" t="n">
+        <v>0.0002991775355383197</v>
+      </c>
+      <c r="EL42" t="n">
+        <v>-0.0002733873621600935</v>
+      </c>
+      <c r="EM42" t="n">
+        <v>-0.0002433722108232672</v>
+      </c>
+      <c r="EN42" t="n">
+        <v>0.000122545304575894</v>
+      </c>
+      <c r="EO42" t="n">
+        <v>-0.0005518730011910833</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
@@ -18154,6 +19288,33 @@
       <c r="EF43" t="n">
         <v>-2.818648594704598e-05</v>
       </c>
+      <c r="EG43" t="n">
+        <v>-6.935462744550591e-06</v>
+      </c>
+      <c r="EH43" t="n">
+        <v>0.0003066369879380915</v>
+      </c>
+      <c r="EI43" t="n">
+        <v>-0.000541444907648625</v>
+      </c>
+      <c r="EJ43" t="n">
+        <v>0.0009570824931106614</v>
+      </c>
+      <c r="EK43" t="n">
+        <v>-0.0006909085752422328</v>
+      </c>
+      <c r="EL43" t="n">
+        <v>0.0005849195947611463</v>
+      </c>
+      <c r="EM43" t="n">
+        <v>-0.0007588671634124466</v>
+      </c>
+      <c r="EN43" t="n">
+        <v>0.0005678699314604074</v>
+      </c>
+      <c r="EO43" t="n">
+        <v>8.736001866083143e-05</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -18566,6 +19727,33 @@
       <c r="EF44" t="n">
         <v>-0.0004273451072585033</v>
       </c>
+      <c r="EG44" t="n">
+        <v>0.0002035853517323716</v>
+      </c>
+      <c r="EH44" t="n">
+        <v>6.759706687198275e-05</v>
+      </c>
+      <c r="EI44" t="n">
+        <v>0.0001312193159925812</v>
+      </c>
+      <c r="EJ44" t="n">
+        <v>0.0008785812502356549</v>
+      </c>
+      <c r="EK44" t="n">
+        <v>0.000373928412004787</v>
+      </c>
+      <c r="EL44" t="n">
+        <v>4.203986264705861e-05</v>
+      </c>
+      <c r="EM44" t="n">
+        <v>0.0004957568969903292</v>
+      </c>
+      <c r="EN44" t="n">
+        <v>-0.0002735465075183185</v>
+      </c>
+      <c r="EO44" t="n">
+        <v>8.558510280920473e-06</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
@@ -18978,6 +20166,33 @@
       <c r="EF45" t="n">
         <v>0.0003189433584029899</v>
       </c>
+      <c r="EG45" t="n">
+        <v>-0.0001288830413948006</v>
+      </c>
+      <c r="EH45" t="n">
+        <v>1.196367112044072e-06</v>
+      </c>
+      <c r="EI45" t="n">
+        <v>0.0002079463437620888</v>
+      </c>
+      <c r="EJ45" t="n">
+        <v>0.0006157626621465795</v>
+      </c>
+      <c r="EK45" t="n">
+        <v>-0.0006269148915585276</v>
+      </c>
+      <c r="EL45" t="n">
+        <v>0.0004279416604671127</v>
+      </c>
+      <c r="EM45" t="n">
+        <v>0.0003699759518287493</v>
+      </c>
+      <c r="EN45" t="n">
+        <v>0.0002865518987462679</v>
+      </c>
+      <c r="EO45" t="n">
+        <v>0.0001011225986449205</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
@@ -19390,6 +20605,33 @@
       <c r="EF46" t="n">
         <v>-0.0003432837847956449</v>
       </c>
+      <c r="EG46" t="n">
+        <v>-0.0004090486613872457</v>
+      </c>
+      <c r="EH46" t="n">
+        <v>3.200228901434343e-05</v>
+      </c>
+      <c r="EI46" t="n">
+        <v>0.0003392514907432087</v>
+      </c>
+      <c r="EJ46" t="n">
+        <v>0.0005240260703960331</v>
+      </c>
+      <c r="EK46" t="n">
+        <v>0.0007004366898257786</v>
+      </c>
+      <c r="EL46" t="n">
+        <v>-0.0004332719758366466</v>
+      </c>
+      <c r="EM46" t="n">
+        <v>0.0002545138036573746</v>
+      </c>
+      <c r="EN46" t="n">
+        <v>-0.0002762038571511027</v>
+      </c>
+      <c r="EO46" t="n">
+        <v>0.0006854556776083598</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
@@ -19802,6 +21044,33 @@
       <c r="EF47" t="n">
         <v>-5.521340725422874e-05</v>
       </c>
+      <c r="EG47" t="n">
+        <v>0.0003267172864731549</v>
+      </c>
+      <c r="EH47" t="n">
+        <v>-6.370650108067366e-05</v>
+      </c>
+      <c r="EI47" t="n">
+        <v>-0.0004458311472586018</v>
+      </c>
+      <c r="EJ47" t="n">
+        <v>8.457947263273979e-05</v>
+      </c>
+      <c r="EK47" t="n">
+        <v>-0.0005816840712160598</v>
+      </c>
+      <c r="EL47" t="n">
+        <v>-6.979958169317513e-05</v>
+      </c>
+      <c r="EM47" t="n">
+        <v>-0.0001862087886248531</v>
+      </c>
+      <c r="EN47" t="n">
+        <v>-0.0004887415554506447</v>
+      </c>
+      <c r="EO47" t="n">
+        <v>0.0002511145247261481</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
@@ -20214,6 +21483,33 @@
       <c r="EF48" t="n">
         <v>0.0004530951620864698</v>
       </c>
+      <c r="EG48" t="n">
+        <v>0.000185161766674824</v>
+      </c>
+      <c r="EH48" t="n">
+        <v>0.0003921443197150154</v>
+      </c>
+      <c r="EI48" t="n">
+        <v>0.0001642344156156383</v>
+      </c>
+      <c r="EJ48" t="n">
+        <v>0.0003924522581133516</v>
+      </c>
+      <c r="EK48" t="n">
+        <v>-0.0001765238217146248</v>
+      </c>
+      <c r="EL48" t="n">
+        <v>0.0003795141640825506</v>
+      </c>
+      <c r="EM48" t="n">
+        <v>-0.000157375436726781</v>
+      </c>
+      <c r="EN48" t="n">
+        <v>-0.0004358103204342711</v>
+      </c>
+      <c r="EO48" t="n">
+        <v>0.0002743356466652358</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
@@ -20626,6 +21922,33 @@
       <c r="EF49" t="n">
         <v>0.000273340663676791</v>
       </c>
+      <c r="EG49" t="n">
+        <v>0.0001264926343012007</v>
+      </c>
+      <c r="EH49" t="n">
+        <v>-0.0004940432797067018</v>
+      </c>
+      <c r="EI49" t="n">
+        <v>-0.0004173187122713529</v>
+      </c>
+      <c r="EJ49" t="n">
+        <v>0.000836885478481264</v>
+      </c>
+      <c r="EK49" t="n">
+        <v>-0.0005329810053105177</v>
+      </c>
+      <c r="EL49" t="n">
+        <v>-0.0003646285419840467</v>
+      </c>
+      <c r="EM49" t="n">
+        <v>-0.0005626813287644694</v>
+      </c>
+      <c r="EN49" t="n">
+        <v>-9.282777224228766e-05</v>
+      </c>
+      <c r="EO49" t="n">
+        <v>0.0006323948927953182</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -21038,6 +22361,33 @@
       <c r="EF50" t="n">
         <v>-0.0004385284385346466</v>
       </c>
+      <c r="EG50" t="n">
+        <v>8.963466254563457e-05</v>
+      </c>
+      <c r="EH50" t="n">
+        <v>6.999433567145275e-05</v>
+      </c>
+      <c r="EI50" t="n">
+        <v>0.0002493673647290251</v>
+      </c>
+      <c r="EJ50" t="n">
+        <v>0.0004227757701222856</v>
+      </c>
+      <c r="EK50" t="n">
+        <v>1.812642273613108e-05</v>
+      </c>
+      <c r="EL50" t="n">
+        <v>0.0005574478044820808</v>
+      </c>
+      <c r="EM50" t="n">
+        <v>0.0008049619946515207</v>
+      </c>
+      <c r="EN50" t="n">
+        <v>0.0003978853541024563</v>
+      </c>
+      <c r="EO50" t="n">
+        <v>0.0009033586958402395</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -21450,6 +22800,33 @@
       <c r="EF51" t="n">
         <v>0.001565911572685152</v>
       </c>
+      <c r="EG51" t="n">
+        <v>-0.0006419812553914994</v>
+      </c>
+      <c r="EH51" t="n">
+        <v>2.61219866892759e-05</v>
+      </c>
+      <c r="EI51" t="n">
+        <v>-0.000387641339958833</v>
+      </c>
+      <c r="EJ51" t="n">
+        <v>0.0002363128660025637</v>
+      </c>
+      <c r="EK51" t="n">
+        <v>0.0001167061537223901</v>
+      </c>
+      <c r="EL51" t="n">
+        <v>-0.0003094537542640552</v>
+      </c>
+      <c r="EM51" t="n">
+        <v>0.0002802645731723175</v>
+      </c>
+      <c r="EN51" t="n">
+        <v>6.902695465882402e-05</v>
+      </c>
+      <c r="EO51" t="n">
+        <v>0.000559466962723576</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
@@ -21862,6 +23239,33 @@
       <c r="EF52" t="n">
         <v>-0.0007997497033951362</v>
       </c>
+      <c r="EG52" t="n">
+        <v>7.928207701013434e-06</v>
+      </c>
+      <c r="EH52" t="n">
+        <v>0.0001400700063207694</v>
+      </c>
+      <c r="EI52" t="n">
+        <v>-0.0003237524515142809</v>
+      </c>
+      <c r="EJ52" t="n">
+        <v>-0.000387319771748551</v>
+      </c>
+      <c r="EK52" t="n">
+        <v>0.0001503183999247426</v>
+      </c>
+      <c r="EL52" t="n">
+        <v>0.0003826308946432988</v>
+      </c>
+      <c r="EM52" t="n">
+        <v>0.0003805438978403686</v>
+      </c>
+      <c r="EN52" t="n">
+        <v>-0.0001528518057387629</v>
+      </c>
+      <c r="EO52" t="n">
+        <v>7.009517702449841e-05</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
@@ -22274,6 +23678,33 @@
       <c r="EF53" t="n">
         <v>-0.0002385468484753517</v>
       </c>
+      <c r="EG53" t="n">
+        <v>7.957590309182194e-05</v>
+      </c>
+      <c r="EH53" t="n">
+        <v>-0.0001607083132633136</v>
+      </c>
+      <c r="EI53" t="n">
+        <v>0.0002122953385939041</v>
+      </c>
+      <c r="EJ53" t="n">
+        <v>-0.000630232793197294</v>
+      </c>
+      <c r="EK53" t="n">
+        <v>-0.0002501068555300634</v>
+      </c>
+      <c r="EL53" t="n">
+        <v>-0.000112984536919214</v>
+      </c>
+      <c r="EM53" t="n">
+        <v>0.0001718493063584958</v>
+      </c>
+      <c r="EN53" t="n">
+        <v>-0.0002145250003078303</v>
+      </c>
+      <c r="EO53" t="n">
+        <v>-0.0004840019603609136</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
@@ -22686,6 +24117,33 @@
       <c r="EF54" t="n">
         <v>-6.248831435939906e-05</v>
       </c>
+      <c r="EG54" t="n">
+        <v>0.0004162086013153043</v>
+      </c>
+      <c r="EH54" t="n">
+        <v>-0.0001018019392802216</v>
+      </c>
+      <c r="EI54" t="n">
+        <v>-0.0001610267114831032</v>
+      </c>
+      <c r="EJ54" t="n">
+        <v>0.0009542383122056464</v>
+      </c>
+      <c r="EK54" t="n">
+        <v>0.0002263473795505178</v>
+      </c>
+      <c r="EL54" t="n">
+        <v>0.0006260792660039982</v>
+      </c>
+      <c r="EM54" t="n">
+        <v>0.0001780402864550723</v>
+      </c>
+      <c r="EN54" t="n">
+        <v>6.707483018431049e-05</v>
+      </c>
+      <c r="EO54" t="n">
+        <v>0.0001650537318358403</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
@@ -23098,6 +24556,33 @@
       <c r="EF55" t="n">
         <v>0.0002236347758834967</v>
       </c>
+      <c r="EG55" t="n">
+        <v>-0.0001176819859658451</v>
+      </c>
+      <c r="EH55" t="n">
+        <v>-0.0005662318044095116</v>
+      </c>
+      <c r="EI55" t="n">
+        <v>0.0005023939695369961</v>
+      </c>
+      <c r="EJ55" t="n">
+        <v>-0.0006061818714009348</v>
+      </c>
+      <c r="EK55" t="n">
+        <v>0.0003723346821438156</v>
+      </c>
+      <c r="EL55" t="n">
+        <v>-0.0002438529746449092</v>
+      </c>
+      <c r="EM55" t="n">
+        <v>0.0001106790635585497</v>
+      </c>
+      <c r="EN55" t="n">
+        <v>0.0003112472410080613</v>
+      </c>
+      <c r="EO55" t="n">
+        <v>-0.0005819773848330101</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
@@ -23510,6 +24995,33 @@
       <c r="EF56" t="n">
         <v>0.0003731076136528344</v>
       </c>
+      <c r="EG56" t="n">
+        <v>0.0001375914573031878</v>
+      </c>
+      <c r="EH56" t="n">
+        <v>6.993605941474357e-05</v>
+      </c>
+      <c r="EI56" t="n">
+        <v>-0.0002298096483830392</v>
+      </c>
+      <c r="EJ56" t="n">
+        <v>0.0003130866453702197</v>
+      </c>
+      <c r="EK56" t="n">
+        <v>0.0009031331526028197</v>
+      </c>
+      <c r="EL56" t="n">
+        <v>0.0003423016842525328</v>
+      </c>
+      <c r="EM56" t="n">
+        <v>-0.0003768131213472969</v>
+      </c>
+      <c r="EN56" t="n">
+        <v>-0.0002088681601790654</v>
+      </c>
+      <c r="EO56" t="n">
+        <v>0.0005624626477001016</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
@@ -23922,6 +25434,33 @@
       <c r="EF57" t="n">
         <v>0.0009481045608463745</v>
       </c>
+      <c r="EG57" t="n">
+        <v>-0.0005122254046412422</v>
+      </c>
+      <c r="EH57" t="n">
+        <v>0.0007606003614402113</v>
+      </c>
+      <c r="EI57" t="n">
+        <v>-0.0002857530705870914</v>
+      </c>
+      <c r="EJ57" t="n">
+        <v>-2.959709116368003e-05</v>
+      </c>
+      <c r="EK57" t="n">
+        <v>-5.992876924487689e-05</v>
+      </c>
+      <c r="EL57" t="n">
+        <v>-0.0002298627022536692</v>
+      </c>
+      <c r="EM57" t="n">
+        <v>-0.0003334834830130973</v>
+      </c>
+      <c r="EN57" t="n">
+        <v>0.0001001004308935904</v>
+      </c>
+      <c r="EO57" t="n">
+        <v>-1.725958235354597e-05</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
@@ -24334,6 +25873,33 @@
       <c r="EF58" t="n">
         <v>0.0003165589525693235</v>
       </c>
+      <c r="EG58" t="n">
+        <v>0.0002824004212964581</v>
+      </c>
+      <c r="EH58" t="n">
+        <v>4.416027469034134e-05</v>
+      </c>
+      <c r="EI58" t="n">
+        <v>0.001358482730802635</v>
+      </c>
+      <c r="EJ58" t="n">
+        <v>-0.00010920367248346</v>
+      </c>
+      <c r="EK58" t="n">
+        <v>5.027730693996091e-07</v>
+      </c>
+      <c r="EL58" t="n">
+        <v>1.647793072656611e-05</v>
+      </c>
+      <c r="EM58" t="n">
+        <v>0.000250320582548369</v>
+      </c>
+      <c r="EN58" t="n">
+        <v>-0.0001686478852143125</v>
+      </c>
+      <c r="EO58" t="n">
+        <v>-0.000166040631102149</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
@@ -24746,6 +26312,33 @@
       <c r="EF59" t="n">
         <v>-0.0006161335667584922</v>
       </c>
+      <c r="EG59" t="n">
+        <v>-0.0007649446799078419</v>
+      </c>
+      <c r="EH59" t="n">
+        <v>0.0004067211193508058</v>
+      </c>
+      <c r="EI59" t="n">
+        <v>-0.0001582255767917928</v>
+      </c>
+      <c r="EJ59" t="n">
+        <v>0.000232535940831724</v>
+      </c>
+      <c r="EK59" t="n">
+        <v>-0.0004058200993366512</v>
+      </c>
+      <c r="EL59" t="n">
+        <v>-0.0001737352587518615</v>
+      </c>
+      <c r="EM59" t="n">
+        <v>-0.0002773913612745815</v>
+      </c>
+      <c r="EN59" t="n">
+        <v>0.0001665769433252251</v>
+      </c>
+      <c r="EO59" t="n">
+        <v>-0.000425868709672983</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
@@ -25158,6 +26751,33 @@
       <c r="EF60" t="n">
         <v>-0.0005981340274114899</v>
       </c>
+      <c r="EG60" t="n">
+        <v>-6.881225392163515e-05</v>
+      </c>
+      <c r="EH60" t="n">
+        <v>-7.931806398353558e-05</v>
+      </c>
+      <c r="EI60" t="n">
+        <v>0.0001376456205743892</v>
+      </c>
+      <c r="EJ60" t="n">
+        <v>-0.000284869031874635</v>
+      </c>
+      <c r="EK60" t="n">
+        <v>0.0001575199958594453</v>
+      </c>
+      <c r="EL60" t="n">
+        <v>0.0003566823316489831</v>
+      </c>
+      <c r="EM60" t="n">
+        <v>0.0005442387720631103</v>
+      </c>
+      <c r="EN60" t="n">
+        <v>0.0003180858554934218</v>
+      </c>
+      <c r="EO60" t="n">
+        <v>-0.0004386155463791397</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
@@ -25570,6 +27190,33 @@
       <c r="EF61" t="n">
         <v>6.106459301946643e-05</v>
       </c>
+      <c r="EG61" t="n">
+        <v>-4.3233175162527e-05</v>
+      </c>
+      <c r="EH61" t="n">
+        <v>-0.0001099197273166652</v>
+      </c>
+      <c r="EI61" t="n">
+        <v>-0.0001200749204688378</v>
+      </c>
+      <c r="EJ61" t="n">
+        <v>0.0002185078588929912</v>
+      </c>
+      <c r="EK61" t="n">
+        <v>-0.0003234155770943659</v>
+      </c>
+      <c r="EL61" t="n">
+        <v>0.0001160199260255013</v>
+      </c>
+      <c r="EM61" t="n">
+        <v>7.928992959271852e-05</v>
+      </c>
+      <c r="EN61" t="n">
+        <v>-0.0003485587820009073</v>
+      </c>
+      <c r="EO61" t="n">
+        <v>0.0004028975108276711</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
@@ -25982,6 +27629,33 @@
       <c r="EF62" t="n">
         <v>-0.001276313759619896</v>
       </c>
+      <c r="EG62" t="n">
+        <v>-0.0005466245525305169</v>
+      </c>
+      <c r="EH62" t="n">
+        <v>-0.0003087965680155236</v>
+      </c>
+      <c r="EI62" t="n">
+        <v>0.0006620397730632277</v>
+      </c>
+      <c r="EJ62" t="n">
+        <v>-0.0008191200405125443</v>
+      </c>
+      <c r="EK62" t="n">
+        <v>-0.0003717301575729692</v>
+      </c>
+      <c r="EL62" t="n">
+        <v>0.0002864261924795386</v>
+      </c>
+      <c r="EM62" t="n">
+        <v>0.0003993163402018496</v>
+      </c>
+      <c r="EN62" t="n">
+        <v>0.0001773019402442344</v>
+      </c>
+      <c r="EO62" t="n">
+        <v>0.0008820779710667637</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
@@ -26394,6 +28068,33 @@
       <c r="EF63" t="n">
         <v>0.0002454231343058666</v>
       </c>
+      <c r="EG63" t="n">
+        <v>-6.637705174128428e-05</v>
+      </c>
+      <c r="EH63" t="n">
+        <v>0.0002967375487816781</v>
+      </c>
+      <c r="EI63" t="n">
+        <v>-0.0006852331624074282</v>
+      </c>
+      <c r="EJ63" t="n">
+        <v>-0.0008830281631269088</v>
+      </c>
+      <c r="EK63" t="n">
+        <v>0.0002598432501663694</v>
+      </c>
+      <c r="EL63" t="n">
+        <v>0.0001517164012714289</v>
+      </c>
+      <c r="EM63" t="n">
+        <v>-0.001101492775145374</v>
+      </c>
+      <c r="EN63" t="n">
+        <v>-0.0001749350777391356</v>
+      </c>
+      <c r="EO63" t="n">
+        <v>0.0002558561165439954</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
@@ -26806,6 +28507,33 @@
       <c r="EF64" t="n">
         <v>0.001138979646112759</v>
       </c>
+      <c r="EG64" t="n">
+        <v>-3.175141814892868e-05</v>
+      </c>
+      <c r="EH64" t="n">
+        <v>-0.0001086373902250415</v>
+      </c>
+      <c r="EI64" t="n">
+        <v>0.0001370440445143117</v>
+      </c>
+      <c r="EJ64" t="n">
+        <v>0.0002568675537144571</v>
+      </c>
+      <c r="EK64" t="n">
+        <v>7.486097143782899e-05</v>
+      </c>
+      <c r="EL64" t="n">
+        <v>0.0001556083980265299</v>
+      </c>
+      <c r="EM64" t="n">
+        <v>0.0006832185180627448</v>
+      </c>
+      <c r="EN64" t="n">
+        <v>-0.0001139116109278859</v>
+      </c>
+      <c r="EO64" t="n">
+        <v>7.478388758563881e-05</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
@@ -27218,6 +28946,33 @@
       <c r="EF65" t="n">
         <v>-0.000701601174705857</v>
       </c>
+      <c r="EG65" t="n">
+        <v>-0.0003646182222674099</v>
+      </c>
+      <c r="EH65" t="n">
+        <v>0.0002877138197163731</v>
+      </c>
+      <c r="EI65" t="n">
+        <v>-0.000201506419294617</v>
+      </c>
+      <c r="EJ65" t="n">
+        <v>-0.0001670221666376648</v>
+      </c>
+      <c r="EK65" t="n">
+        <v>-0.0003231295959427172</v>
+      </c>
+      <c r="EL65" t="n">
+        <v>1.917329471368134e-05</v>
+      </c>
+      <c r="EM65" t="n">
+        <v>0.0001634014921947369</v>
+      </c>
+      <c r="EN65" t="n">
+        <v>0.0001717993789860373</v>
+      </c>
+      <c r="EO65" t="n">
+        <v>0.0001556266484588065</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
@@ -27630,6 +29385,33 @@
       <c r="EF66" t="n">
         <v>-0.0003162223890438298</v>
       </c>
+      <c r="EG66" t="n">
+        <v>-0.000215618011491614</v>
+      </c>
+      <c r="EH66" t="n">
+        <v>9.167212548177872e-06</v>
+      </c>
+      <c r="EI66" t="n">
+        <v>-0.0003447735483064207</v>
+      </c>
+      <c r="EJ66" t="n">
+        <v>0.0001762273017060778</v>
+      </c>
+      <c r="EK66" t="n">
+        <v>0.0001271107698617158</v>
+      </c>
+      <c r="EL66" t="n">
+        <v>-4.547443311331278e-05</v>
+      </c>
+      <c r="EM66" t="n">
+        <v>0.0001558729736146347</v>
+      </c>
+      <c r="EN66" t="n">
+        <v>0.000389742990977382</v>
+      </c>
+      <c r="EO66" t="n">
+        <v>8.133174763713669e-05</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
@@ -28042,6 +29824,33 @@
       <c r="EF67" t="n">
         <v>0.0008408636894579047</v>
       </c>
+      <c r="EG67" t="n">
+        <v>-0.0005017002499929646</v>
+      </c>
+      <c r="EH67" t="n">
+        <v>-7.722642927454615e-05</v>
+      </c>
+      <c r="EI67" t="n">
+        <v>-0.0002075440980888743</v>
+      </c>
+      <c r="EJ67" t="n">
+        <v>4.642900512941139e-05</v>
+      </c>
+      <c r="EK67" t="n">
+        <v>0.0002177516068524454</v>
+      </c>
+      <c r="EL67" t="n">
+        <v>-0.000477757093205966</v>
+      </c>
+      <c r="EM67" t="n">
+        <v>0.0008074061572482805</v>
+      </c>
+      <c r="EN67" t="n">
+        <v>-0.0002612579258567393</v>
+      </c>
+      <c r="EO67" t="n">
+        <v>-0.0002443091201627112</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
@@ -28454,6 +30263,33 @@
       <c r="EF68" t="n">
         <v>0.0008787602392228422</v>
       </c>
+      <c r="EG68" t="n">
+        <v>0.0001157152827264696</v>
+      </c>
+      <c r="EH68" t="n">
+        <v>0.0003320811490183928</v>
+      </c>
+      <c r="EI68" t="n">
+        <v>0.0001723871892860274</v>
+      </c>
+      <c r="EJ68" t="n">
+        <v>0.0003538618229264046</v>
+      </c>
+      <c r="EK68" t="n">
+        <v>-0.0002631392670426891</v>
+      </c>
+      <c r="EL68" t="n">
+        <v>0.0004320798082364519</v>
+      </c>
+      <c r="EM68" t="n">
+        <v>-0.0002431497981927322</v>
+      </c>
+      <c r="EN68" t="n">
+        <v>-0.0006245350957563289</v>
+      </c>
+      <c r="EO68" t="n">
+        <v>0.001043849713433076</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
@@ -28866,6 +30702,33 @@
       <c r="EF69" t="n">
         <v>-0.001085994268997581</v>
       </c>
+      <c r="EG69" t="n">
+        <v>-8.342971618446882e-06</v>
+      </c>
+      <c r="EH69" t="n">
+        <v>-0.0001970633581009906</v>
+      </c>
+      <c r="EI69" t="n">
+        <v>0.0003727007727487575</v>
+      </c>
+      <c r="EJ69" t="n">
+        <v>0.0004491503143420061</v>
+      </c>
+      <c r="EK69" t="n">
+        <v>0.0003395020983827379</v>
+      </c>
+      <c r="EL69" t="n">
+        <v>-0.0001403577679628398</v>
+      </c>
+      <c r="EM69" t="n">
+        <v>-0.0003340944719187888</v>
+      </c>
+      <c r="EN69" t="n">
+        <v>-0.0004854380285284066</v>
+      </c>
+      <c r="EO69" t="n">
+        <v>-9.693338040683841e-05</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
@@ -29278,6 +31141,33 @@
       <c r="EF70" t="n">
         <v>6.74027135492139e-05</v>
       </c>
+      <c r="EG70" t="n">
+        <v>0.0001731024001365711</v>
+      </c>
+      <c r="EH70" t="n">
+        <v>0.0003758612639028769</v>
+      </c>
+      <c r="EI70" t="n">
+        <v>-0.0002417224508803884</v>
+      </c>
+      <c r="EJ70" t="n">
+        <v>4.790554724820595e-05</v>
+      </c>
+      <c r="EK70" t="n">
+        <v>-9.527837314315946e-05</v>
+      </c>
+      <c r="EL70" t="n">
+        <v>-0.0002301570862393021</v>
+      </c>
+      <c r="EM70" t="n">
+        <v>-8.783079211482914e-06</v>
+      </c>
+      <c r="EN70" t="n">
+        <v>-2.961312816296413e-06</v>
+      </c>
+      <c r="EO70" t="n">
+        <v>3.955778703002011e-05</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
@@ -29690,6 +31580,33 @@
       <c r="EF71" t="n">
         <v>-0.0005348993261886648</v>
       </c>
+      <c r="EG71" t="n">
+        <v>3.128036957811275e-05</v>
+      </c>
+      <c r="EH71" t="n">
+        <v>-0.0002697530630300093</v>
+      </c>
+      <c r="EI71" t="n">
+        <v>-0.0004294600407241944</v>
+      </c>
+      <c r="EJ71" t="n">
+        <v>0.001442760946499533</v>
+      </c>
+      <c r="EK71" t="n">
+        <v>-0.0001052493888256123</v>
+      </c>
+      <c r="EL71" t="n">
+        <v>0.0001708153666282186</v>
+      </c>
+      <c r="EM71" t="n">
+        <v>0.0003527427909677527</v>
+      </c>
+      <c r="EN71" t="n">
+        <v>-0.0007248969936295424</v>
+      </c>
+      <c r="EO71" t="n">
+        <v>-0.0001387528820746553</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
@@ -30102,6 +32019,33 @@
       <c r="EF72" t="n">
         <v>0.0007071410466714667</v>
       </c>
+      <c r="EG72" t="n">
+        <v>8.857275438423073e-05</v>
+      </c>
+      <c r="EH72" t="n">
+        <v>-1.962667767685389e-05</v>
+      </c>
+      <c r="EI72" t="n">
+        <v>0.0003061158955368626</v>
+      </c>
+      <c r="EJ72" t="n">
+        <v>-0.001247220965250762</v>
+      </c>
+      <c r="EK72" t="n">
+        <v>-0.0001338417039065121</v>
+      </c>
+      <c r="EL72" t="n">
+        <v>0.0002210827400617177</v>
+      </c>
+      <c r="EM72" t="n">
+        <v>0.0001514192200851028</v>
+      </c>
+      <c r="EN72" t="n">
+        <v>0.0002555167860638363</v>
+      </c>
+      <c r="EO72" t="n">
+        <v>0.0005435427607860532</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
@@ -30514,6 +32458,33 @@
       <c r="EF73" t="n">
         <v>0.0001441542846567501</v>
       </c>
+      <c r="EG73" t="n">
+        <v>-0.0007057215535635208</v>
+      </c>
+      <c r="EH73" t="n">
+        <v>-0.0001759599110862098</v>
+      </c>
+      <c r="EI73" t="n">
+        <v>9.64308724249463e-06</v>
+      </c>
+      <c r="EJ73" t="n">
+        <v>0.0001846920598573831</v>
+      </c>
+      <c r="EK73" t="n">
+        <v>0.0003005652954435334</v>
+      </c>
+      <c r="EL73" t="n">
+        <v>0.0003147728146188911</v>
+      </c>
+      <c r="EM73" t="n">
+        <v>0.0003009947445278272</v>
+      </c>
+      <c r="EN73" t="n">
+        <v>2.103500209571507e-05</v>
+      </c>
+      <c r="EO73" t="n">
+        <v>0.0001132335192988165</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
@@ -30926,6 +32897,33 @@
       <c r="EF74" t="n">
         <v>-5.394426965388277e-05</v>
       </c>
+      <c r="EG74" t="n">
+        <v>-0.0006722145407618285</v>
+      </c>
+      <c r="EH74" t="n">
+        <v>0.0002461957366168832</v>
+      </c>
+      <c r="EI74" t="n">
+        <v>-0.0002144802075392249</v>
+      </c>
+      <c r="EJ74" t="n">
+        <v>0.0003894792965635219</v>
+      </c>
+      <c r="EK74" t="n">
+        <v>0.0003388954705894065</v>
+      </c>
+      <c r="EL74" t="n">
+        <v>0.0005508147280828268</v>
+      </c>
+      <c r="EM74" t="n">
+        <v>3.461055996289986e-05</v>
+      </c>
+      <c r="EN74" t="n">
+        <v>9.035659607015134e-05</v>
+      </c>
+      <c r="EO74" t="n">
+        <v>-0.0001320254561480994</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
@@ -31338,6 +33336,33 @@
       <c r="EF75" t="n">
         <v>-2.282345166015887e-05</v>
       </c>
+      <c r="EG75" t="n">
+        <v>5.200018514273097e-05</v>
+      </c>
+      <c r="EH75" t="n">
+        <v>0.0008411513583954644</v>
+      </c>
+      <c r="EI75" t="n">
+        <v>-0.0003633651227339385</v>
+      </c>
+      <c r="EJ75" t="n">
+        <v>3.292101612473175e-05</v>
+      </c>
+      <c r="EK75" t="n">
+        <v>-0.0002620328807410033</v>
+      </c>
+      <c r="EL75" t="n">
+        <v>0.0001656867050741084</v>
+      </c>
+      <c r="EM75" t="n">
+        <v>-0.0001644847946504768</v>
+      </c>
+      <c r="EN75" t="n">
+        <v>0.0004236289863293052</v>
+      </c>
+      <c r="EO75" t="n">
+        <v>-2.701402791771557e-05</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
@@ -31750,6 +33775,33 @@
       <c r="EF76" t="n">
         <v>-0.0002545513669449662</v>
       </c>
+      <c r="EG76" t="n">
+        <v>4.523696740044159e-05</v>
+      </c>
+      <c r="EH76" t="n">
+        <v>0.0001426278167375727</v>
+      </c>
+      <c r="EI76" t="n">
+        <v>-0.0004348852417876969</v>
+      </c>
+      <c r="EJ76" t="n">
+        <v>-0.0001648179189910337</v>
+      </c>
+      <c r="EK76" t="n">
+        <v>-0.0001084544249518871</v>
+      </c>
+      <c r="EL76" t="n">
+        <v>-0.000332705021753199</v>
+      </c>
+      <c r="EM76" t="n">
+        <v>0.0002183210625990029</v>
+      </c>
+      <c r="EN76" t="n">
+        <v>4.589635055296526e-05</v>
+      </c>
+      <c r="EO76" t="n">
+        <v>-6.949596147975967e-05</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
@@ -32162,6 +34214,33 @@
       <c r="EF77" t="n">
         <v>0.0001659202974675367</v>
       </c>
+      <c r="EG77" t="n">
+        <v>5.060332536466206e-05</v>
+      </c>
+      <c r="EH77" t="n">
+        <v>0.0002694742154467633</v>
+      </c>
+      <c r="EI77" t="n">
+        <v>-0.0003696905673749029</v>
+      </c>
+      <c r="EJ77" t="n">
+        <v>0.0001908712064473406</v>
+      </c>
+      <c r="EK77" t="n">
+        <v>-0.0002913156999753141</v>
+      </c>
+      <c r="EL77" t="n">
+        <v>0.0002855693464169917</v>
+      </c>
+      <c r="EM77" t="n">
+        <v>0.000542440778902531</v>
+      </c>
+      <c r="EN77" t="n">
+        <v>0.0002702028985588356</v>
+      </c>
+      <c r="EO77" t="n">
+        <v>-0.0002420010917525417</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
@@ -32574,6 +34653,33 @@
       <c r="EF78" t="n">
         <v>0.0001286458680418434</v>
       </c>
+      <c r="EG78" t="n">
+        <v>-0.0001414770213301608</v>
+      </c>
+      <c r="EH78" t="n">
+        <v>-0.001070563724031359</v>
+      </c>
+      <c r="EI78" t="n">
+        <v>-0.0005293298507016431</v>
+      </c>
+      <c r="EJ78" t="n">
+        <v>0.0006064054752830117</v>
+      </c>
+      <c r="EK78" t="n">
+        <v>-2.64691551077334e-05</v>
+      </c>
+      <c r="EL78" t="n">
+        <v>0.0002374609737323397</v>
+      </c>
+      <c r="EM78" t="n">
+        <v>2.079279989608551e-05</v>
+      </c>
+      <c r="EN78" t="n">
+        <v>-0.0006164021901025052</v>
+      </c>
+      <c r="EO78" t="n">
+        <v>-0.0001357107057167184</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
@@ -32986,6 +35092,33 @@
       <c r="EF79" t="n">
         <v>-0.0004644678250791401</v>
       </c>
+      <c r="EG79" t="n">
+        <v>-0.0002484037239529613</v>
+      </c>
+      <c r="EH79" t="n">
+        <v>6.772814602129529e-05</v>
+      </c>
+      <c r="EI79" t="n">
+        <v>-0.0002778065220265802</v>
+      </c>
+      <c r="EJ79" t="n">
+        <v>-1.927575342897114e-05</v>
+      </c>
+      <c r="EK79" t="n">
+        <v>-0.0003246312230427151</v>
+      </c>
+      <c r="EL79" t="n">
+        <v>-0.0002629352209755353</v>
+      </c>
+      <c r="EM79" t="n">
+        <v>6.789385719407903e-05</v>
+      </c>
+      <c r="EN79" t="n">
+        <v>0.0001783959542915881</v>
+      </c>
+      <c r="EO79" t="n">
+        <v>-0.0001251521682590351</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
@@ -33398,6 +35531,33 @@
       <c r="EF80" t="n">
         <v>-0.0001437322604580515</v>
       </c>
+      <c r="EG80" t="n">
+        <v>-0.0002627903938474674</v>
+      </c>
+      <c r="EH80" t="n">
+        <v>3.685015254362156e-05</v>
+      </c>
+      <c r="EI80" t="n">
+        <v>0.001002558398678133</v>
+      </c>
+      <c r="EJ80" t="n">
+        <v>-0.0004201220555710705</v>
+      </c>
+      <c r="EK80" t="n">
+        <v>0.0001388242015192276</v>
+      </c>
+      <c r="EL80" t="n">
+        <v>8.504534737419078e-05</v>
+      </c>
+      <c r="EM80" t="n">
+        <v>0.0002157713494170821</v>
+      </c>
+      <c r="EN80" t="n">
+        <v>0.0001575385298959731</v>
+      </c>
+      <c r="EO80" t="n">
+        <v>-0.0007297786187017152</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
@@ -33810,6 +35970,33 @@
       <c r="EF81" t="n">
         <v>-0.0002434231997501257</v>
       </c>
+      <c r="EG81" t="n">
+        <v>-0.0009520742919040259</v>
+      </c>
+      <c r="EH81" t="n">
+        <v>0.000532382948939869</v>
+      </c>
+      <c r="EI81" t="n">
+        <v>4.957861945698028e-05</v>
+      </c>
+      <c r="EJ81" t="n">
+        <v>0.0002254262096830217</v>
+      </c>
+      <c r="EK81" t="n">
+        <v>1.61061005421459e-06</v>
+      </c>
+      <c r="EL81" t="n">
+        <v>0.0001453024954329862</v>
+      </c>
+      <c r="EM81" t="n">
+        <v>0.0004103297164164132</v>
+      </c>
+      <c r="EN81" t="n">
+        <v>0.0002501746671388361</v>
+      </c>
+      <c r="EO81" t="n">
+        <v>-7.399709317290615e-05</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
@@ -34222,6 +36409,33 @@
       <c r="EF82" t="n">
         <v>-0.0002546591638221685</v>
       </c>
+      <c r="EG82" t="n">
+        <v>-0.0004119240926776513</v>
+      </c>
+      <c r="EH82" t="n">
+        <v>-0.0003980407844235145</v>
+      </c>
+      <c r="EI82" t="n">
+        <v>-0.0003008281547138836</v>
+      </c>
+      <c r="EJ82" t="n">
+        <v>-0.0004278786311537885</v>
+      </c>
+      <c r="EK82" t="n">
+        <v>-0.0002321559333164913</v>
+      </c>
+      <c r="EL82" t="n">
+        <v>0.0004725634126376832</v>
+      </c>
+      <c r="EM82" t="n">
+        <v>-0.0005206727177480275</v>
+      </c>
+      <c r="EN82" t="n">
+        <v>0.000118305391346496</v>
+      </c>
+      <c r="EO82" t="n">
+        <v>-9.860596076194383e-05</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
@@ -34634,6 +36848,33 @@
       <c r="EF83" t="n">
         <v>0.0003442442101011522</v>
       </c>
+      <c r="EG83" t="n">
+        <v>0.0006103559638166445</v>
+      </c>
+      <c r="EH83" t="n">
+        <v>0.0002242285531597332</v>
+      </c>
+      <c r="EI83" t="n">
+        <v>-0.0003531434786196996</v>
+      </c>
+      <c r="EJ83" t="n">
+        <v>3.393004775631425e-05</v>
+      </c>
+      <c r="EK83" t="n">
+        <v>5.376510269528012e-05</v>
+      </c>
+      <c r="EL83" t="n">
+        <v>-0.0005193908277014714</v>
+      </c>
+      <c r="EM83" t="n">
+        <v>0.0003864427120188196</v>
+      </c>
+      <c r="EN83" t="n">
+        <v>-8.534818785044251e-05</v>
+      </c>
+      <c r="EO83" t="n">
+        <v>-0.0004681679009106432</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
@@ -35046,6 +37287,33 @@
       <c r="EF84" t="n">
         <v>0.0002019818649294791</v>
       </c>
+      <c r="EG84" t="n">
+        <v>-0.0003494974789610694</v>
+      </c>
+      <c r="EH84" t="n">
+        <v>-0.000239962284258155</v>
+      </c>
+      <c r="EI84" t="n">
+        <v>0.0002384609800092363</v>
+      </c>
+      <c r="EJ84" t="n">
+        <v>-0.000313694853229407</v>
+      </c>
+      <c r="EK84" t="n">
+        <v>-0.0001752002976829203</v>
+      </c>
+      <c r="EL84" t="n">
+        <v>2.155893242061779e-05</v>
+      </c>
+      <c r="EM84" t="n">
+        <v>0.0002983738352817511</v>
+      </c>
+      <c r="EN84" t="n">
+        <v>0.0003991498142319472</v>
+      </c>
+      <c r="EO84" t="n">
+        <v>-4.14838732467615e-05</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
@@ -35458,6 +37726,33 @@
       <c r="EF85" t="n">
         <v>-9.579541665338809e-05</v>
       </c>
+      <c r="EG85" t="n">
+        <v>-0.0005966184592836044</v>
+      </c>
+      <c r="EH85" t="n">
+        <v>-0.0001892224853747848</v>
+      </c>
+      <c r="EI85" t="n">
+        <v>0.0004204382114334493</v>
+      </c>
+      <c r="EJ85" t="n">
+        <v>0.0002878434926945062</v>
+      </c>
+      <c r="EK85" t="n">
+        <v>-0.0002623543878979007</v>
+      </c>
+      <c r="EL85" t="n">
+        <v>0.0002378193302181586</v>
+      </c>
+      <c r="EM85" t="n">
+        <v>-0.0003101924537620704</v>
+      </c>
+      <c r="EN85" t="n">
+        <v>-6.421231295483665e-05</v>
+      </c>
+      <c r="EO85" t="n">
+        <v>-0.0003864809409037662</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
@@ -35870,6 +38165,33 @@
       <c r="EF86" t="n">
         <v>-0.001934281179060804</v>
       </c>
+      <c r="EG86" t="n">
+        <v>-0.002520550922524123</v>
+      </c>
+      <c r="EH86" t="n">
+        <v>-0.002682042168665077</v>
+      </c>
+      <c r="EI86" t="n">
+        <v>-0.0003653084915917759</v>
+      </c>
+      <c r="EJ86" t="n">
+        <v>-7.064023102465455e-05</v>
+      </c>
+      <c r="EK86" t="n">
+        <v>0.001401010367638733</v>
+      </c>
+      <c r="EL86" t="n">
+        <v>0.002272570879123137</v>
+      </c>
+      <c r="EM86" t="n">
+        <v>-3.742591639266379e-06</v>
+      </c>
+      <c r="EN86" t="n">
+        <v>-0.0001841770784452024</v>
+      </c>
+      <c r="EO86" t="n">
+        <v>-0.001174680712960452</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>